<commit_message>
Limpieza de HTML viejos y render con nombres actualizados
</commit_message>
<xml_diff>
--- a/data/DBCA_Frijol/DBCA_frijol.xlsx
+++ b/data/DBCA_Frijol/DBCA_frijol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailudesedu-my.sharepoint.com/personal/fr_ortiz_mail_udes_edu_co/Documents/1_2025B_INFO SEMESTRAL/2025B_GR_PMD_Manual R/DBCA_Frijo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R-Proyectos\r-para-mi\data\DBCA_Frijol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_C9A847FD29553A672ECE86FD319A23BBBB7D5489" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB2EDE29-DB95-462A-A226-2803328D8910}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F63176-6EB4-4432-8731-3EC2ABF0582E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +117,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{71322A8C-13F2-4389-BA1A-3E9B5BA74946}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -660,17 +662,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="F123" sqref="F123"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection sqref="A1:C121"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -692,7 +694,7 @@
         <v>51.49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -703,7 +705,7 @@
         <v>49.59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -714,7 +716,7 @@
         <v>51.94</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -725,7 +727,7 @@
         <v>54.57</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -736,7 +738,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -747,7 +749,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -758,7 +760,7 @@
         <v>54.74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -769,7 +771,7 @@
         <v>52.3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -780,7 +782,7 @@
         <v>48.59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -791,7 +793,7 @@
         <v>51.63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -802,7 +804,7 @@
         <v>53.61</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -813,7 +815,7 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -824,7 +826,7 @@
         <v>55.73</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -835,7 +837,7 @@
         <v>49.26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -846,7 +848,7 @@
         <v>49.83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -857,7 +859,7 @@
         <v>53.31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -868,7 +870,7 @@
         <v>51.96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -879,7 +881,7 @@
         <v>55.94</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -890,7 +892,7 @@
         <v>52.28</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
@@ -901,7 +903,7 @@
         <v>50.76</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -912,7 +914,7 @@
         <v>64.400000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -923,7 +925,7 @@
         <v>59.32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -934,7 +936,7 @@
         <v>60.2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -945,7 +947,7 @@
         <v>55.73</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -956,7 +958,7 @@
         <v>58.37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -967,7 +969,7 @@
         <v>60.33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -978,7 +980,7 @@
         <v>56.55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -989,7 +991,7 @@
         <v>61.13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1000,7 +1002,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>59.12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1022,7 +1024,7 @@
         <v>63.19</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1033,7 +1035,7 @@
         <v>70.56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>64.959999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1055,7 +1057,7 @@
         <v>61.83</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1066,7 +1068,7 @@
         <v>67.47</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -1077,7 +1079,7 @@
         <v>61.34</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1090,7 @@
         <v>65.63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>59.12</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>61.02</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>65.59</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>10</v>
       </c>
@@ -1132,7 +1134,7 @@
         <v>52.22</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -1143,7 +1145,7 @@
         <v>50.51</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -1154,7 +1156,7 @@
         <v>49.65</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>10</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>10</v>
       </c>
@@ -1176,7 +1178,7 @@
         <v>45.56</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1189,7 @@
         <v>47.84</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>10</v>
       </c>
@@ -1198,7 +1200,7 @@
         <v>48.62</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -1209,7 +1211,7 @@
         <v>53.17</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>10</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>51.03</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>10</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>44.71</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1244,7 @@
         <v>55.97</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>11</v>
       </c>
@@ -1253,7 +1255,7 @@
         <v>53.84</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1266,7 @@
         <v>52.97</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>11</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>56.84</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>11</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>58.09</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>11</v>
       </c>
@@ -1297,7 +1299,7 @@
         <v>57.79</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>11</v>
       </c>
@@ -1308,7 +1310,7 @@
         <v>52.48</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>11</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>54.07</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>11</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>55.99</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>11</v>
       </c>
@@ -1341,7 +1343,7 @@
         <v>57.93</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -1352,7 +1354,7 @@
         <v>58.56</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -1363,7 +1365,7 @@
         <v>59.44</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>56.68</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>12</v>
       </c>
@@ -1385,7 +1387,7 @@
         <v>56.41</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>62.44</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -1407,7 +1409,7 @@
         <v>64.069999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>12</v>
       </c>
@@ -1418,7 +1420,7 @@
         <v>59.78</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>12</v>
       </c>
@@ -1429,7 +1431,7 @@
         <v>63.01</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -1440,7 +1442,7 @@
         <v>61.08</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>12</v>
       </c>
@@ -1451,7 +1453,7 @@
         <v>58.06</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1464,7 @@
         <v>66.08</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>13</v>
       </c>
@@ -1473,7 +1475,7 @@
         <v>69.61</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1486,7 @@
         <v>64.89</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>13</v>
       </c>
@@ -1495,7 +1497,7 @@
         <v>69.69</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>13</v>
       </c>
@@ -1506,7 +1508,7 @@
         <v>57.14</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>13</v>
       </c>
@@ -1517,7 +1519,7 @@
         <v>67.47</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>13</v>
       </c>
@@ -1528,7 +1530,7 @@
         <v>65.260000000000005</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>13</v>
       </c>
@@ -1539,7 +1541,7 @@
         <v>64.099999999999994</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>65.28</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -1561,7 +1563,7 @@
         <v>59.04</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>10</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>49.34</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>10</v>
       </c>
@@ -1583,7 +1585,7 @@
         <v>51.07</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>10</v>
       </c>
@@ -1594,7 +1596,7 @@
         <v>54.43</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>10</v>
       </c>
@@ -1605,7 +1607,7 @@
         <v>48.45</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>10</v>
       </c>
@@ -1616,7 +1618,7 @@
         <v>47.57</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>10</v>
       </c>
@@ -1627,7 +1629,7 @@
         <v>48.49</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1640,7 @@
         <v>52.75</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>10</v>
       </c>
@@ -1649,7 +1651,7 @@
         <v>50.99</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>10</v>
       </c>
@@ -1660,7 +1662,7 @@
         <v>48.41</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>10</v>
       </c>
@@ -1671,7 +1673,7 @@
         <v>51.54</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>11</v>
       </c>
@@ -1682,7 +1684,7 @@
         <v>55.29</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>11</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>57.91</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>11</v>
       </c>
@@ -1704,7 +1706,7 @@
         <v>52.89</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>11</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>54.02</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>11</v>
       </c>
@@ -1726,7 +1728,7 @@
         <v>53.82</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>11</v>
       </c>
@@ -1737,7 +1739,7 @@
         <v>50.61</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>11</v>
       </c>
@@ -1748,7 +1750,7 @@
         <v>55.89</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>11</v>
       </c>
@@ -1759,7 +1761,7 @@
         <v>55.78</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>11</v>
       </c>
@@ -1770,7 +1772,7 @@
         <v>55.02</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>11</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>54.3</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>12</v>
       </c>
@@ -1792,7 +1794,7 @@
         <v>55.75</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>12</v>
       </c>
@@ -1803,7 +1805,7 @@
         <v>58.74</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>12</v>
       </c>
@@ -1814,7 +1816,7 @@
         <v>58.97</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>12</v>
       </c>
@@ -1825,7 +1827,7 @@
         <v>57.59</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +1838,7 @@
         <v>59.52</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>12</v>
       </c>
@@ -1847,7 +1849,7 @@
         <v>61.21</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>12</v>
       </c>
@@ -1858,7 +1860,7 @@
         <v>65.66</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>12</v>
       </c>
@@ -1869,7 +1871,7 @@
         <v>60.52</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -1880,7 +1882,7 @@
         <v>60.77</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>12</v>
       </c>
@@ -1891,7 +1893,7 @@
         <v>59.78</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>13</v>
       </c>
@@ -1902,7 +1904,7 @@
         <v>59.24</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>13</v>
       </c>
@@ -1913,7 +1915,7 @@
         <v>64.92</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>13</v>
       </c>
@@ -1924,7 +1926,7 @@
         <v>65.180000000000007</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>13</v>
       </c>
@@ -1935,7 +1937,7 @@
         <v>72.39</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>13</v>
       </c>
@@ -1946,7 +1948,7 @@
         <v>64.42</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -1957,7 +1959,7 @@
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>13</v>
       </c>
@@ -1968,7 +1970,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>13</v>
       </c>
@@ -1979,7 +1981,7 @@
         <v>61.49</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>13</v>
       </c>
@@ -1990,7 +1992,7 @@
         <v>68.430000000000007</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>13</v>
       </c>
@@ -2015,9 +2017,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2028,7 +2030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7.4355000000000002</v>
       </c>
@@ -2050,9 +2052,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2063,7 +2065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2074,7 +2076,7 @@
         <v>0.6392349940723121</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2085,7 +2087,7 @@
         <v>0.45476325835616838</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2096,7 +2098,7 @@
         <v>0.40781858014630978</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2118,9 +2120,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2128,7 +2130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2136,7 +2138,7 @@
         <v>50.296666666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>54.259333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2152,7 +2154,7 @@
         <v>59.713000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>